<commit_message>
Prepare key points in excel && Add some learning materials
Signed-off-by: Shelwin Wei <shelwin.wei@sap.com>
</commit_message>
<xml_diff>
--- a/MeMi Learning Plan.xlsx
+++ b/MeMi Learning Plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1. Grid Usage Billing" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,195 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+  <si>
+    <t>BAdI: ISU_BI_UPDATE</t>
+  </si>
+  <si>
+    <t>Settlement Quantity &amp; Grid Usage Quanity</t>
+  </si>
+  <si>
+    <t>Overtake &amp; Undertake</t>
+  </si>
+  <si>
+    <t>MeMi Period (Synchronous Begin and End &amp; Asynchronous Begin and End)</t>
+  </si>
+  <si>
+    <t>MSCONS</t>
+  </si>
+  <si>
+    <t>INVOIC</t>
+  </si>
+  <si>
+    <t>MeMi Price</t>
+  </si>
+  <si>
+    <t>Reverse Charge Type</t>
+  </si>
+  <si>
+    <t>Energy Tax</t>
+  </si>
+  <si>
+    <t>Billable Item -&gt; Billing Document -&gt; Invoicing Document -&gt; Posting Document -&gt; Clearing Document</t>
+  </si>
+  <si>
+    <t>Split MeMi Document</t>
+  </si>
+  <si>
+    <t>EDM Query</t>
+  </si>
+  <si>
+    <t>Single Process &amp; Mass Process</t>
+  </si>
+  <si>
+    <t>Reveral Origin (Manual/Mass Reversal/Grid Usage)</t>
+  </si>
+  <si>
+    <t>Reversal MSCONS</t>
+  </si>
+  <si>
+    <t>Reversal INVOIC</t>
+  </si>
+  <si>
+    <t>What fields are copied from original?</t>
+  </si>
+  <si>
+    <t>Deadline step 200 in mass process</t>
+  </si>
+  <si>
+    <t>Deadline step 200 in mass reversal process</t>
+  </si>
+  <si>
+    <t>When to create billable item?</t>
+  </si>
+  <si>
+    <t>When to create reversal billable item?</t>
+  </si>
+  <si>
+    <t>Check Whether Reversal Process is Completed</t>
+  </si>
+  <si>
+    <t>/IDXMM/MGV_DETIF</t>
+  </si>
+  <si>
+    <t>/IDXMM/MGV_GAMA</t>
+  </si>
+  <si>
+    <t>When to create MGV detail information entry?</t>
+  </si>
+  <si>
+    <t>When to update MGV detail information entry?</t>
+  </si>
+  <si>
+    <t>Correction Reports</t>
+  </si>
+  <si>
+    <t>Split Settlement Item</t>
+  </si>
+  <si>
+    <t>Consumption Item</t>
+  </si>
+  <si>
+    <t>Rating -&gt; Billing -&gt; Invoicing/Posting</t>
+  </si>
+  <si>
+    <t>SSQNOT</t>
+  </si>
+  <si>
+    <t>MGV Billing Process</t>
+  </si>
+  <si>
+    <t>MGV Reversal Billing Process</t>
+  </si>
+  <si>
+    <t>PAN type</t>
+  </si>
+  <si>
+    <t>FP05/FPY1</t>
+  </si>
+  <si>
+    <t>FP06/FPMA</t>
+  </si>
+  <si>
+    <t>FP07/FP08</t>
+  </si>
+  <si>
+    <t>Payment Reversal -&gt; Status Rollback (MM) / Distribution Lot (GU)</t>
+  </si>
+  <si>
+    <t>Process Control</t>
+  </si>
+  <si>
+    <t>TINVINV_LINA</t>
+  </si>
+  <si>
+    <t>Billing Process &amp; Subprocess (MeMi/MGV)</t>
+  </si>
+  <si>
+    <t>Invoicing Process (MM/MG)</t>
+  </si>
+  <si>
+    <t>Main Transaction &amp; Subtransaction</t>
+  </si>
+  <si>
+    <t>Source Transaction Type &amp; BIT Class &amp; Subprocess &amp; Billable Item Type</t>
+  </si>
+  <si>
+    <t>Billing Item Type (YME)</t>
+  </si>
+  <si>
+    <t>Consumptioin Item ID Type</t>
+  </si>
+  <si>
+    <t>Reverse Consumption Item/Billable Item/Billing Document/Invoicing Document</t>
+  </si>
+  <si>
+    <t>Send/Receive Subscription Request (4031/4032)</t>
+  </si>
+  <si>
+    <t>Send Allocation List</t>
+  </si>
+  <si>
+    <t>BAdI</t>
+  </si>
+  <si>
+    <t>Reference Month</t>
+  </si>
+  <si>
+    <t>FPVA</t>
+  </si>
+  <si>
+    <t>FPVB</t>
+  </si>
+  <si>
+    <t>FPVC</t>
+  </si>
+  <si>
+    <t>Dunning Level</t>
+  </si>
+  <si>
+    <t>Dunning History</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -67,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -351,7 +527,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -361,14 +537,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -376,14 +633,55 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -391,74 +689,250 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>